<commit_message>
Cambio de logica en similitud flexible al 90%
</commit_message>
<xml_diff>
--- a/ADRpy/analisis/Data/Datos_aeronaves.xlsx
+++ b/ADRpy/analisis/Data/Datos_aeronaves.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfef281a55a6378e/Tesis/ADRpy-VTOL/ADRpy/analisis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{7EA34CBB-A0A6-412D-86CF-3FCA05BB820E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9A114FC-9C90-45C5-99D7-B1CD5F2C9C1F}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{7EA34CBB-A0A6-412D-86CF-3FCA05BB820E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44073584-DCF9-41DB-97B9-7D4EAF5044E5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{10BA835C-0312-4895-8548-B5BE30C3D790}"/>
   </bookViews>
@@ -33,11 +33,24 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>Ezequiel Delpino</author>
     <author>tc={340A3259-C3B5-485D-AF11-616C5CE93D9F}</author>
-    <author>Ezequiel Delpino</author>
   </authors>
   <commentList>
-    <comment ref="AA19" authorId="0" shapeId="0" xr:uid="{111E6D55-2CFD-45CC-A397-2A3EAC164856}">
+    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{0B0F7441-BF84-4215-9345-9E5C070EA683}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tiempo máximo de vuelo con velocidad de menor consumo de combustible, aproximadamente un 20% mayor al tiempo maximo de vuelo a velocidad crucero</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA19" authorId="1" shapeId="0" xr:uid="{111E6D55-2CFD-45CC-A397-2A3EAC164856}">
       <text>
         <r>
           <rPr>
@@ -54,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D32" authorId="1" shapeId="0" xr:uid="{685BE65D-47BF-49CA-B248-3D62DC2C801E}">
+    <comment ref="D32" authorId="0" shapeId="0" xr:uid="{685BE65D-47BF-49CA-B248-3D62DC2C801E}">
       <text>
         <r>
           <rPr>
@@ -78,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A38" authorId="1" shapeId="0" xr:uid="{0AB079C1-9CF0-43C9-A5A3-9443BF0C2678}">
+    <comment ref="A38" authorId="0" shapeId="0" xr:uid="{0AB079C1-9CF0-43C9-A5A3-9443BF0C2678}">
       <text>
         <r>
           <rPr>
@@ -105,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A39" authorId="1" shapeId="0" xr:uid="{C992F673-0EF7-40A6-9C21-1C5CF8C16E89}">
+    <comment ref="A39" authorId="0" shapeId="0" xr:uid="{C992F673-0EF7-40A6-9C21-1C5CF8C16E89}">
       <text>
         <r>
           <rPr>
@@ -133,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A40" authorId="1" shapeId="0" xr:uid="{ED649FF3-DBD5-44B0-893A-9BA7FE8B1512}">
+    <comment ref="A40" authorId="0" shapeId="0" xr:uid="{ED649FF3-DBD5-44B0-893A-9BA7FE8B1512}">
       <text>
         <r>
           <rPr>
@@ -161,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A43" authorId="1" shapeId="0" xr:uid="{4BB1D5BA-63A0-4C32-8F4E-91D34F7636D9}">
+    <comment ref="A43" authorId="0" shapeId="0" xr:uid="{4BB1D5BA-63A0-4C32-8F4E-91D34F7636D9}">
       <text>
         <r>
           <rPr>
@@ -255,7 +268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3940" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3942" uniqueCount="646">
   <si>
     <t>Tabla para análisis estadístico de aeronaves existentes</t>
   </si>
@@ -2181,6 +2194,18 @@
   </si>
   <si>
     <t>31.0</t>
+  </si>
+  <si>
+    <t>Aerosonde Mk. 4.8 VTOL FTUAS</t>
+  </si>
+  <si>
+    <t>Aerosonde Mk. 4.8 Fixed wing</t>
+  </si>
+  <si>
+    <t>Aerosonde Mk. 4.7 Fixed Wing</t>
+  </si>
+  <si>
+    <t>Aerosonde Mk. 4.7 VTOL</t>
   </si>
 </sst>
 </file>
@@ -2191,7 +2216,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0##"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2393,8 +2418,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2531,6 +2564,12 @@
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -2777,7 +2816,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="248">
+  <cellXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
@@ -3371,6 +3410,15 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="26" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="21" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3485,8 +3533,11 @@
     <xf numFmtId="0" fontId="18" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3494,14 +3545,7 @@
     <cellStyle name="Hyperlink" xfId="2" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="51">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF7030A0"/>
-      </font>
-    </dxf>
+  <dxfs count="50">
     <dxf>
       <font>
         <b/>
@@ -5362,7 +5406,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{627D0B30-6438-472E-AB25-67DDB56F6D16}" name="Tabla2" displayName="Tabla2" ref="D4:BA62" totalsRowShown="0" headerRowDxfId="50" headerRowBorderDxfId="49" tableBorderDxfId="48" totalsRowBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{627D0B30-6438-472E-AB25-67DDB56F6D16}" name="Tabla2" displayName="Tabla2" ref="D4:BA62" totalsRowShown="0" headerRowDxfId="49" headerRowBorderDxfId="48" tableBorderDxfId="47" totalsRowBorderDxfId="46">
   <autoFilter ref="D4:BA62" xr:uid="{627D0B30-6438-472E-AB25-67DDB56F6D16}">
     <filterColumn colId="0">
       <filters>
@@ -5385,49 +5429,49 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="50">
-    <tableColumn id="1" xr3:uid="{D1ECE87B-AEE4-4B09-81CE-E239013CB1DA}" name="Modelo" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{B150F19E-80AB-4FA5-909F-F23889FD36F0}" name="Stalker XE" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{B657D819-977D-4FAE-B95C-190841DCDF1D}" name="Stalker VXE30" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{7B634440-B964-44B8-9358-3453733D1ECB}" name="Aerosonde Mk. 4.7 Fixed Wing" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{5FA3CF84-28F9-4A9D-BFE5-5DF2A2A7AE27}" name="Aerosonde Mk. 4.7 VTOL" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{C86E8C48-5D0A-46E6-AE84-E8E631388EC0}" name="Aerosonde Mk. 4.8 Fixed wing" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{91BC1274-8C76-4D0E-A159-065FEFFDE1C7}" name="Aerosonde Mk. 4.8 VTOL FTUAS" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{BE77BC37-4C69-4DC5-BE80-F49ECD523CA7}" name="AAI Aerosonde" dataDxfId="39"/>
-    <tableColumn id="9" xr3:uid="{ABD69575-3136-404C-8D22-41B2FB240688}" name="Fulmar X" dataDxfId="38"/>
-    <tableColumn id="10" xr3:uid="{C51EFB4D-3890-4A20-A72F-01E7C9647DA8}" name="Orbiter 4" dataDxfId="37"/>
-    <tableColumn id="11" xr3:uid="{919E422E-01F3-401D-A87C-19535757C40E}" name="Orbiter 3" dataDxfId="36"/>
-    <tableColumn id="12" xr3:uid="{BCA9E281-A8D6-48DD-AF52-0D0CB95265FD}" name="Mantis" dataDxfId="35"/>
-    <tableColumn id="13" xr3:uid="{1EEFD3B3-FBFF-4883-A540-8E806152616D}" name="ScanEagle" dataDxfId="34"/>
-    <tableColumn id="14" xr3:uid="{BC038E9C-F2DD-45E0-9CDA-053E39037BA2}" name="Integrator" dataDxfId="33"/>
-    <tableColumn id="15" xr3:uid="{9A7D16A2-F7E6-4F42-BE4A-090A4533A2C8}" name="Integrator VTOL" dataDxfId="32"/>
-    <tableColumn id="16" xr3:uid="{F8E426AD-9AC8-4D27-B695-1D70C117D603}" name="Integrator Extended Range (ER)" dataDxfId="31"/>
-    <tableColumn id="17" xr3:uid="{64D96181-A953-4552-9F3C-4384227E2853}" name="ScanEagle 3" dataDxfId="30"/>
-    <tableColumn id="18" xr3:uid="{B6CC6305-8C71-4B68-A166-7A7D21D368DD}" name="RQ Nan 21A Blackjack" dataDxfId="29"/>
-    <tableColumn id="19" xr3:uid="{4E9AD48D-987E-4566-A20E-166DFEBB4E93}" name="DeltaQuad Evo" dataDxfId="28"/>
-    <tableColumn id="20" xr3:uid="{BFC89D69-561A-4F8A-846A-D21C43CDE803}" name="DeltaQuad Pro #MAP" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{D1ECE87B-AEE4-4B09-81CE-E239013CB1DA}" name="Modelo" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{B150F19E-80AB-4FA5-909F-F23889FD36F0}" name="Stalker XE" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{B657D819-977D-4FAE-B95C-190841DCDF1D}" name="Stalker VXE30" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{7B634440-B964-44B8-9358-3453733D1ECB}" name="Aerosonde Mk. 4.7 Fixed Wing" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{5FA3CF84-28F9-4A9D-BFE5-5DF2A2A7AE27}" name="Aerosonde Mk. 4.7 VTOL" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{C86E8C48-5D0A-46E6-AE84-E8E631388EC0}" name="Aerosonde Mk. 4.8 Fixed wing" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{91BC1274-8C76-4D0E-A159-065FEFFDE1C7}" name="Aerosonde Mk. 4.8 VTOL FTUAS" dataDxfId="39"/>
+    <tableColumn id="8" xr3:uid="{BE77BC37-4C69-4DC5-BE80-F49ECD523CA7}" name="AAI Aerosonde" dataDxfId="38"/>
+    <tableColumn id="9" xr3:uid="{ABD69575-3136-404C-8D22-41B2FB240688}" name="Fulmar X" dataDxfId="37"/>
+    <tableColumn id="10" xr3:uid="{C51EFB4D-3890-4A20-A72F-01E7C9647DA8}" name="Orbiter 4" dataDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{919E422E-01F3-401D-A87C-19535757C40E}" name="Orbiter 3" dataDxfId="35"/>
+    <tableColumn id="12" xr3:uid="{BCA9E281-A8D6-48DD-AF52-0D0CB95265FD}" name="Mantis" dataDxfId="34"/>
+    <tableColumn id="13" xr3:uid="{1EEFD3B3-FBFF-4883-A540-8E806152616D}" name="ScanEagle" dataDxfId="33"/>
+    <tableColumn id="14" xr3:uid="{BC038E9C-F2DD-45E0-9CDA-053E39037BA2}" name="Integrator" dataDxfId="32"/>
+    <tableColumn id="15" xr3:uid="{9A7D16A2-F7E6-4F42-BE4A-090A4533A2C8}" name="Integrator VTOL" dataDxfId="31"/>
+    <tableColumn id="16" xr3:uid="{F8E426AD-9AC8-4D27-B695-1D70C117D603}" name="Integrator Extended Range (ER)" dataDxfId="30"/>
+    <tableColumn id="17" xr3:uid="{64D96181-A953-4552-9F3C-4384227E2853}" name="ScanEagle 3" dataDxfId="29"/>
+    <tableColumn id="18" xr3:uid="{B6CC6305-8C71-4B68-A166-7A7D21D368DD}" name="RQ Nan 21A Blackjack" dataDxfId="28"/>
+    <tableColumn id="19" xr3:uid="{4E9AD48D-987E-4566-A20E-166DFEBB4E93}" name="DeltaQuad Evo" dataDxfId="27"/>
+    <tableColumn id="20" xr3:uid="{BFC89D69-561A-4F8A-846A-D21C43CDE803}" name="DeltaQuad Pro #MAP" dataDxfId="26"/>
     <tableColumn id="21" xr3:uid="{E36A8EFD-988E-495A-B23B-71427691C95A}" name="DeltaQuad Pro #CARGO"/>
-    <tableColumn id="22" xr3:uid="{1EE075D4-462A-4E8D-BCC8-A7BDA4A4B505}" name="V21" dataDxfId="26"/>
-    <tableColumn id="23" xr3:uid="{D0B4673E-75BF-4698-B44A-1176BBD13D07}" name="V25" dataDxfId="25"/>
-    <tableColumn id="24" xr3:uid="{90C79FBD-04BB-42F2-A67C-7F8D6C726450}" name="V32" dataDxfId="24"/>
-    <tableColumn id="25" xr3:uid="{D09F91B1-AEDD-4957-9763-BBD7075475BD}" name="V35" dataDxfId="23"/>
-    <tableColumn id="26" xr3:uid="{2AAF05BF-E31C-4EB1-9EBE-CF900CE11144}" name="V39" dataDxfId="22"/>
-    <tableColumn id="27" xr3:uid="{7C7F911E-355C-4C8D-8452-DB7936F813AE}" name="Volitation VT370" dataDxfId="21"/>
-    <tableColumn id="28" xr3:uid="{00FF4733-D375-4BB4-9D5A-E79554C0D826}" name="Skyeye 2600" dataDxfId="20"/>
-    <tableColumn id="29" xr3:uid="{E783A2B9-ABFF-4516-A79A-B6F1B236BE02}" name="Skyeye 2930 VTOL" dataDxfId="19"/>
-    <tableColumn id="30" xr3:uid="{1F4A0EF2-2A7C-41FE-88D2-EDD9288EF5C6}" name="Skyeye 3600" dataDxfId="18"/>
-    <tableColumn id="31" xr3:uid="{63E3AAC7-F47A-44E1-AF56-EB776C4A964B}" name="Skyeye 3600 VTOL" dataDxfId="17"/>
-    <tableColumn id="32" xr3:uid="{08EB6092-3AB0-4B3E-A0F8-25E710675352}" name="Skyeye 5000" dataDxfId="16"/>
-    <tableColumn id="33" xr3:uid="{C98D7A4A-6B67-4DB1-812C-620C76F40C93}" name="Skyeye 5000 VTOL" dataDxfId="15"/>
-    <tableColumn id="34" xr3:uid="{24A21FCC-F5B4-4B64-B41E-B1E3585BE976}" name="Skyeye 5000 VTOL octo" dataDxfId="14"/>
-    <tableColumn id="35" xr3:uid="{8248873A-D5CC-4D22-A5B4-128DA101196C}" name="Volitation VT510" dataDxfId="13"/>
-    <tableColumn id="36" xr3:uid="{863BAA6B-2B95-41CB-89BE-3DDAD5B9BD3F}" name="Ascend" dataDxfId="12"/>
-    <tableColumn id="37" xr3:uid="{DA353A44-CAA6-4BDB-BEEC-EC0DB3B2E471}" name="Transition" dataDxfId="11"/>
-    <tableColumn id="38" xr3:uid="{C072C93A-0AF8-4A4E-A368-C21FB1814132}" name="Reach" dataDxfId="10"/>
-    <tableColumn id="39" xr3:uid="{421CAA57-5F5C-42CC-99AD-C4FE9B36C3D0}" name="WingtraOne GEN II" dataDxfId="9"/>
-    <tableColumn id="40" xr3:uid="{CF744639-59A2-4E40-957E-4EC2C0BF6E31}" name="Trinity Pro" dataDxfId="8"/>
-    <tableColumn id="41" xr3:uid="{088A0092-4E62-498E-B5F2-3255EBA7A234}" name="Vector" dataDxfId="7"/>
-    <tableColumn id="42" xr3:uid="{B7A406EA-3140-4166-9471-61350F754C9A}" name="Scorpion" dataDxfId="6"/>
-    <tableColumn id="43" xr3:uid="{7FF61606-E053-4A43-82BB-518EDCE11C2B}" name="Trinity F90+" dataDxfId="5"/>
+    <tableColumn id="22" xr3:uid="{1EE075D4-462A-4E8D-BCC8-A7BDA4A4B505}" name="V21" dataDxfId="25"/>
+    <tableColumn id="23" xr3:uid="{D0B4673E-75BF-4698-B44A-1176BBD13D07}" name="V25" dataDxfId="24"/>
+    <tableColumn id="24" xr3:uid="{90C79FBD-04BB-42F2-A67C-7F8D6C726450}" name="V32" dataDxfId="23"/>
+    <tableColumn id="25" xr3:uid="{D09F91B1-AEDD-4957-9763-BBD7075475BD}" name="V35" dataDxfId="22"/>
+    <tableColumn id="26" xr3:uid="{2AAF05BF-E31C-4EB1-9EBE-CF900CE11144}" name="V39" dataDxfId="21"/>
+    <tableColumn id="27" xr3:uid="{7C7F911E-355C-4C8D-8452-DB7936F813AE}" name="Volitation VT370" dataDxfId="20"/>
+    <tableColumn id="28" xr3:uid="{00FF4733-D375-4BB4-9D5A-E79554C0D826}" name="Skyeye 2600" dataDxfId="19"/>
+    <tableColumn id="29" xr3:uid="{E783A2B9-ABFF-4516-A79A-B6F1B236BE02}" name="Skyeye 2930 VTOL" dataDxfId="18"/>
+    <tableColumn id="30" xr3:uid="{1F4A0EF2-2A7C-41FE-88D2-EDD9288EF5C6}" name="Skyeye 3600" dataDxfId="17"/>
+    <tableColumn id="31" xr3:uid="{63E3AAC7-F47A-44E1-AF56-EB776C4A964B}" name="Skyeye 3600 VTOL" dataDxfId="16"/>
+    <tableColumn id="32" xr3:uid="{08EB6092-3AB0-4B3E-A0F8-25E710675352}" name="Skyeye 5000" dataDxfId="15"/>
+    <tableColumn id="33" xr3:uid="{C98D7A4A-6B67-4DB1-812C-620C76F40C93}" name="Skyeye 5000 VTOL" dataDxfId="14"/>
+    <tableColumn id="34" xr3:uid="{24A21FCC-F5B4-4B64-B41E-B1E3585BE976}" name="Skyeye 5000 VTOL octo" dataDxfId="13"/>
+    <tableColumn id="35" xr3:uid="{8248873A-D5CC-4D22-A5B4-128DA101196C}" name="Volitation VT510" dataDxfId="12"/>
+    <tableColumn id="36" xr3:uid="{863BAA6B-2B95-41CB-89BE-3DDAD5B9BD3F}" name="Ascend" dataDxfId="11"/>
+    <tableColumn id="37" xr3:uid="{DA353A44-CAA6-4BDB-BEEC-EC0DB3B2E471}" name="Transition" dataDxfId="10"/>
+    <tableColumn id="38" xr3:uid="{C072C93A-0AF8-4A4E-A368-C21FB1814132}" name="Reach" dataDxfId="9"/>
+    <tableColumn id="39" xr3:uid="{421CAA57-5F5C-42CC-99AD-C4FE9B36C3D0}" name="WingtraOne GEN II" dataDxfId="8"/>
+    <tableColumn id="40" xr3:uid="{CF744639-59A2-4E40-957E-4EC2C0BF6E31}" name="Trinity Pro" dataDxfId="7"/>
+    <tableColumn id="41" xr3:uid="{088A0092-4E62-498E-B5F2-3255EBA7A234}" name="Vector" dataDxfId="6"/>
+    <tableColumn id="42" xr3:uid="{B7A406EA-3140-4166-9471-61350F754C9A}" name="Scorpion" dataDxfId="5"/>
+    <tableColumn id="43" xr3:uid="{7FF61606-E053-4A43-82BB-518EDCE11C2B}" name="Trinity F90+" dataDxfId="4"/>
     <tableColumn id="44" xr3:uid="{900F05A7-0C34-48C8-8EAC-3F43E451FD8B}" name="CWNan007"/>
     <tableColumn id="45" xr3:uid="{8B950811-DA7F-4D86-88AB-8C19AC0500DE}" name="CWNan15"/>
     <tableColumn id="46" xr3:uid="{99660027-DEF1-4E8A-9727-89F3CFB994E6}" name="CWNan25"/>
@@ -5745,17 +5789,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78AB5BED-A5EE-454B-B1C7-2585704905C8}">
-  <dimension ref="A1:AP79"/>
+  <dimension ref="A1:AP78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection activeCell="A9" sqref="A9"/>
-      <selection pane="topRight" activeCell="C49" sqref="C49"/>
+      <selection pane="topRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.33203125" style="112" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.44140625" style="112" customWidth="1"/>
     <col min="2" max="8" width="15.77734375" style="23" customWidth="1"/>
     <col min="9" max="21" width="15.77734375" style="113" customWidth="1"/>
     <col min="22" max="38" width="15.77734375" style="23" customWidth="1"/>
@@ -5772,17 +5816,17 @@
       <c r="C1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>478</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>480</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>481</v>
+      <c r="D1" s="210" t="s">
+        <v>644</v>
+      </c>
+      <c r="E1" s="211" t="s">
+        <v>645</v>
+      </c>
+      <c r="F1" s="211" t="s">
+        <v>643</v>
+      </c>
+      <c r="G1" s="211" t="s">
+        <v>642</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>23</v>
@@ -6752,7 +6796,7 @@
       <c r="D9" s="124">
         <v>3</v>
       </c>
-      <c r="E9" s="124">
+      <c r="E9" s="251">
         <v>3</v>
       </c>
       <c r="F9" s="124">
@@ -7231,8 +7275,8 @@
       <c r="I13" s="117">
         <v>800</v>
       </c>
-      <c r="J13" s="117">
-        <v>150</v>
+      <c r="J13" s="117" t="s">
+        <v>457</v>
       </c>
       <c r="K13" s="117">
         <v>50</v>
@@ -7255,8 +7299,8 @@
       <c r="Q13" s="117" t="s">
         <v>457</v>
       </c>
-      <c r="R13" s="117">
-        <v>92.6</v>
+      <c r="R13" s="117" t="s">
+        <v>457</v>
       </c>
       <c r="S13" s="117">
         <v>270</v>
@@ -9571,7 +9615,7 @@
       <c r="G33" s="129" t="s">
         <v>457</v>
       </c>
-      <c r="H33" s="173">
+      <c r="H33" s="250">
         <v>1280</v>
       </c>
       <c r="I33" s="128" t="s">
@@ -10664,7 +10708,7 @@
       <c r="V42" s="168">
         <v>1</v>
       </c>
-      <c r="W42" s="247">
+      <c r="W42" s="209">
         <v>1</v>
       </c>
       <c r="X42" s="168">
@@ -12771,7 +12815,49 @@
     <row r="65" spans="2:42" ht="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="66" spans="2:42" ht="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="67" spans="2:42" ht="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" spans="2:42" ht="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="2:42" s="112" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="23"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="113"/>
+      <c r="J68" s="113"/>
+      <c r="K68" s="113"/>
+      <c r="L68" s="113"/>
+      <c r="M68" s="113"/>
+      <c r="N68" s="113"/>
+      <c r="O68" s="113"/>
+      <c r="P68" s="113"/>
+      <c r="Q68" s="113"/>
+      <c r="R68" s="113"/>
+      <c r="S68" s="113"/>
+      <c r="T68" s="113"/>
+      <c r="U68" s="113"/>
+      <c r="V68" s="23"/>
+      <c r="W68" s="23"/>
+      <c r="X68" s="23"/>
+      <c r="Y68" s="23"/>
+      <c r="Z68" s="23"/>
+      <c r="AA68" s="23"/>
+      <c r="AB68" s="23"/>
+      <c r="AC68" s="23"/>
+      <c r="AD68" s="23"/>
+      <c r="AE68" s="23"/>
+      <c r="AF68" s="23"/>
+      <c r="AG68" s="23"/>
+      <c r="AH68" s="23"/>
+      <c r="AI68" s="23"/>
+      <c r="AJ68" s="23"/>
+      <c r="AK68" s="23"/>
+      <c r="AL68" s="23"/>
+      <c r="AM68" s="23"/>
+      <c r="AN68" s="23"/>
+      <c r="AO68" s="23"/>
+      <c r="AP68" s="23"/>
+    </row>
     <row r="69" spans="2:42" s="112" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="23"/>
       <c r="C69" s="23"/>
@@ -13202,52 +13288,9 @@
       <c r="AO78" s="23"/>
       <c r="AP78" s="23"/>
     </row>
-    <row r="79" spans="2:42" s="112" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="23"/>
-      <c r="C79" s="23"/>
-      <c r="D79" s="23"/>
-      <c r="E79" s="23"/>
-      <c r="F79" s="23"/>
-      <c r="G79" s="23"/>
-      <c r="H79" s="23"/>
-      <c r="I79" s="113"/>
-      <c r="J79" s="113"/>
-      <c r="K79" s="113"/>
-      <c r="L79" s="113"/>
-      <c r="M79" s="113"/>
-      <c r="N79" s="113"/>
-      <c r="O79" s="113"/>
-      <c r="P79" s="113"/>
-      <c r="Q79" s="113"/>
-      <c r="R79" s="113"/>
-      <c r="S79" s="113"/>
-      <c r="T79" s="113"/>
-      <c r="U79" s="113"/>
-      <c r="V79" s="23"/>
-      <c r="W79" s="23"/>
-      <c r="X79" s="23"/>
-      <c r="Y79" s="23"/>
-      <c r="Z79" s="23"/>
-      <c r="AA79" s="23"/>
-      <c r="AB79" s="23"/>
-      <c r="AC79" s="23"/>
-      <c r="AD79" s="23"/>
-      <c r="AE79" s="23"/>
-      <c r="AF79" s="23"/>
-      <c r="AG79" s="23"/>
-      <c r="AH79" s="23"/>
-      <c r="AI79" s="23"/>
-      <c r="AJ79" s="23"/>
-      <c r="AK79" s="23"/>
-      <c r="AL79" s="23"/>
-      <c r="AM79" s="23"/>
-      <c r="AN79" s="23"/>
-      <c r="AO79" s="23"/>
-      <c r="AP79" s="23"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:AL37">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>NOT(ISNUMBER(B2))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13415,57 +13458,57 @@
       <c r="D2" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="215" t="s">
+      <c r="E2" s="218" t="s">
         <v>443</v>
       </c>
-      <c r="F2" s="216"/>
-      <c r="G2" s="216"/>
-      <c r="H2" s="216"/>
-      <c r="I2" s="216"/>
-      <c r="J2" s="216"/>
-      <c r="K2" s="216"/>
-      <c r="L2" s="216"/>
-      <c r="M2" s="216"/>
-      <c r="N2" s="216"/>
-      <c r="O2" s="216"/>
-      <c r="P2" s="216"/>
-      <c r="Q2" s="216"/>
-      <c r="R2" s="216"/>
-      <c r="S2" s="216"/>
-      <c r="T2" s="216"/>
-      <c r="U2" s="216"/>
-      <c r="V2" s="216"/>
-      <c r="W2" s="216"/>
-      <c r="X2" s="216"/>
-      <c r="Y2" s="216"/>
-      <c r="Z2" s="216"/>
-      <c r="AA2" s="216"/>
-      <c r="AB2" s="216"/>
-      <c r="AC2" s="216"/>
-      <c r="AD2" s="216"/>
-      <c r="AE2" s="216"/>
-      <c r="AF2" s="216"/>
-      <c r="AG2" s="216"/>
-      <c r="AH2" s="216"/>
-      <c r="AI2" s="216"/>
-      <c r="AJ2" s="216"/>
-      <c r="AK2" s="216"/>
-      <c r="AL2" s="216"/>
-      <c r="AM2" s="216"/>
-      <c r="AN2" s="216"/>
-      <c r="AO2" s="216"/>
-      <c r="AP2" s="216"/>
-      <c r="AQ2" s="216"/>
-      <c r="AR2" s="216"/>
-      <c r="AS2" s="216"/>
-      <c r="AT2" s="216"/>
-      <c r="AU2" s="216"/>
-      <c r="AV2" s="216"/>
-      <c r="AW2" s="216"/>
-      <c r="AX2" s="216"/>
-      <c r="AY2" s="216"/>
-      <c r="AZ2" s="216"/>
-      <c r="BA2" s="217"/>
+      <c r="F2" s="219"/>
+      <c r="G2" s="219"/>
+      <c r="H2" s="219"/>
+      <c r="I2" s="219"/>
+      <c r="J2" s="219"/>
+      <c r="K2" s="219"/>
+      <c r="L2" s="219"/>
+      <c r="M2" s="219"/>
+      <c r="N2" s="219"/>
+      <c r="O2" s="219"/>
+      <c r="P2" s="219"/>
+      <c r="Q2" s="219"/>
+      <c r="R2" s="219"/>
+      <c r="S2" s="219"/>
+      <c r="T2" s="219"/>
+      <c r="U2" s="219"/>
+      <c r="V2" s="219"/>
+      <c r="W2" s="219"/>
+      <c r="X2" s="219"/>
+      <c r="Y2" s="219"/>
+      <c r="Z2" s="219"/>
+      <c r="AA2" s="219"/>
+      <c r="AB2" s="219"/>
+      <c r="AC2" s="219"/>
+      <c r="AD2" s="219"/>
+      <c r="AE2" s="219"/>
+      <c r="AF2" s="219"/>
+      <c r="AG2" s="219"/>
+      <c r="AH2" s="219"/>
+      <c r="AI2" s="219"/>
+      <c r="AJ2" s="219"/>
+      <c r="AK2" s="219"/>
+      <c r="AL2" s="219"/>
+      <c r="AM2" s="219"/>
+      <c r="AN2" s="219"/>
+      <c r="AO2" s="219"/>
+      <c r="AP2" s="219"/>
+      <c r="AQ2" s="219"/>
+      <c r="AR2" s="219"/>
+      <c r="AS2" s="219"/>
+      <c r="AT2" s="219"/>
+      <c r="AU2" s="219"/>
+      <c r="AV2" s="219"/>
+      <c r="AW2" s="219"/>
+      <c r="AX2" s="219"/>
+      <c r="AY2" s="219"/>
+      <c r="AZ2" s="219"/>
+      <c r="BA2" s="220"/>
       <c r="BB2" s="72"/>
       <c r="BC2" s="72"/>
       <c r="BD2" s="72"/>
@@ -13777,7 +13820,7 @@
       </c>
     </row>
     <row r="5" spans="1:57" s="78" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="212" t="s">
+      <c r="A5" s="215" t="s">
         <v>60</v>
       </c>
       <c r="B5" s="90" t="s">
@@ -13907,7 +13950,7 @@
       <c r="BA5" s="174"/>
     </row>
     <row r="6" spans="1:57" s="78" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="213"/>
+      <c r="A6" s="216"/>
       <c r="B6" s="90" t="s">
         <v>66</v>
       </c>
@@ -14032,7 +14075,7 @@
       <c r="BA6" s="174"/>
     </row>
     <row r="7" spans="1:57" s="78" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="213"/>
+      <c r="A7" s="216"/>
       <c r="B7" s="90" t="s">
         <v>71</v>
       </c>
@@ -14157,7 +14200,7 @@
       <c r="BA7" s="174"/>
     </row>
     <row r="8" spans="1:57" s="78" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="213"/>
+      <c r="A8" s="216"/>
       <c r="B8" s="90" t="s">
         <v>75</v>
       </c>
@@ -14311,7 +14354,7 @@
       <c r="BA8" s="174"/>
     </row>
     <row r="9" spans="1:57" s="78" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="213"/>
+      <c r="A9" s="216"/>
       <c r="B9" s="90" t="s">
         <v>79</v>
       </c>
@@ -14436,7 +14479,7 @@
       <c r="BA9" s="174"/>
     </row>
     <row r="10" spans="1:57" s="78" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="214"/>
+      <c r="A10" s="217"/>
       <c r="B10" s="90" t="s">
         <v>83</v>
       </c>
@@ -14574,7 +14617,7 @@
       <c r="BA10" s="174"/>
     </row>
     <row r="11" spans="1:57" s="94" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="218" t="s">
+      <c r="A11" s="221" t="s">
         <v>85</v>
       </c>
       <c r="B11" s="92" t="s">
@@ -14702,7 +14745,7 @@
       <c r="BA11" s="175"/>
     </row>
     <row r="12" spans="1:57" s="94" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="219"/>
+      <c r="A12" s="222"/>
       <c r="B12" s="92" t="s">
         <v>89</v>
       </c>
@@ -14833,7 +14876,7 @@
       <c r="BA12" s="175"/>
     </row>
     <row r="13" spans="1:57" s="94" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="219"/>
+      <c r="A13" s="222"/>
       <c r="B13" s="92" t="s">
         <v>91</v>
       </c>
@@ -14958,7 +15001,7 @@
       <c r="BA13" s="175"/>
     </row>
     <row r="14" spans="1:57" s="94" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="219"/>
+      <c r="A14" s="222"/>
       <c r="B14" s="92" t="s">
         <v>93</v>
       </c>
@@ -15083,7 +15126,7 @@
       <c r="BA14" s="175"/>
     </row>
     <row r="15" spans="1:57" s="94" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="219"/>
+      <c r="A15" s="222"/>
       <c r="B15" s="92" t="s">
         <v>95</v>
       </c>
@@ -15208,7 +15251,7 @@
       <c r="BA15" s="175"/>
     </row>
     <row r="16" spans="1:57" s="142" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="220"/>
+      <c r="A16" s="223"/>
       <c r="B16" s="139" t="s">
         <v>98</v>
       </c>
@@ -15333,7 +15376,7 @@
       <c r="BA16" s="176"/>
     </row>
     <row r="17" spans="1:53" s="97" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="221" t="s">
+      <c r="A17" s="224" t="s">
         <v>100</v>
       </c>
       <c r="B17" s="95" t="s">
@@ -15460,7 +15503,7 @@
       <c r="BA17" s="177"/>
     </row>
     <row r="18" spans="1:53" s="97" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="222"/>
+      <c r="A18" s="225"/>
       <c r="B18" s="95" t="s">
         <v>104</v>
       </c>
@@ -15585,7 +15628,7 @@
       <c r="BA18" s="177"/>
     </row>
     <row r="19" spans="1:53" s="97" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="222"/>
+      <c r="A19" s="225"/>
       <c r="B19" s="95" t="s">
         <v>108</v>
       </c>
@@ -15710,7 +15753,7 @@
       <c r="BA19" s="177"/>
     </row>
     <row r="20" spans="1:53" s="97" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="222"/>
+      <c r="A20" s="225"/>
       <c r="B20" s="95" t="s">
         <v>110</v>
       </c>
@@ -15835,7 +15878,7 @@
       <c r="BA20" s="177"/>
     </row>
     <row r="21" spans="1:53" s="97" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="222"/>
+      <c r="A21" s="225"/>
       <c r="B21" s="95" t="s">
         <v>66</v>
       </c>
@@ -15960,7 +16003,7 @@
       <c r="BA21" s="177"/>
     </row>
     <row r="22" spans="1:53" s="97" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="223"/>
+      <c r="A22" s="226"/>
       <c r="B22" s="95" t="s">
         <v>113</v>
       </c>
@@ -16085,7 +16128,7 @@
       <c r="BA22" s="177"/>
     </row>
     <row r="23" spans="1:53" s="86" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="224" t="s">
+      <c r="A23" s="227" t="s">
         <v>115</v>
       </c>
       <c r="B23" s="108"/>
@@ -16210,7 +16253,7 @@
       <c r="BA23" s="178"/>
     </row>
     <row r="24" spans="1:53" s="86" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="225"/>
+      <c r="A24" s="228"/>
       <c r="B24" s="108"/>
       <c r="C24" s="86" t="s">
         <v>63</v>
@@ -16335,7 +16378,7 @@
       <c r="BA24" s="178"/>
     </row>
     <row r="25" spans="1:53" s="86" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="225"/>
+      <c r="A25" s="228"/>
       <c r="B25" s="108"/>
       <c r="C25" s="88" t="s">
         <v>70</v>
@@ -16458,7 +16501,7 @@
       <c r="BA25" s="178"/>
     </row>
     <row r="26" spans="1:53" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="225"/>
+      <c r="A26" s="228"/>
       <c r="B26" s="108"/>
       <c r="C26" s="88" t="s">
         <v>149</v>
@@ -16581,7 +16624,7 @@
       <c r="BA26" s="178"/>
     </row>
     <row r="27" spans="1:53" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="225"/>
+      <c r="A27" s="228"/>
       <c r="B27" s="108"/>
       <c r="C27" s="88" t="s">
         <v>77</v>
@@ -16704,7 +16747,7 @@
       <c r="BA27" s="178"/>
     </row>
     <row r="28" spans="1:53" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="225"/>
+      <c r="A28" s="228"/>
       <c r="B28" s="108"/>
       <c r="C28" s="88" t="s">
         <v>70</v>
@@ -16827,7 +16870,7 @@
       <c r="BA28" s="178"/>
     </row>
     <row r="29" spans="1:53" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="225"/>
+      <c r="A29" s="228"/>
       <c r="B29" s="108"/>
       <c r="C29" s="88" t="s">
         <v>70</v>
@@ -16954,7 +16997,7 @@
       <c r="BA29" s="178"/>
     </row>
     <row r="30" spans="1:53" s="86" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="225"/>
+      <c r="A30" s="228"/>
       <c r="B30" s="108"/>
       <c r="C30" s="88" t="s">
         <v>70</v>
@@ -17081,7 +17124,7 @@
       <c r="BA30" s="178"/>
     </row>
     <row r="31" spans="1:53" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="225"/>
+      <c r="A31" s="228"/>
       <c r="B31" s="108"/>
       <c r="C31" s="88" t="s">
         <v>77</v>
@@ -17208,7 +17251,7 @@
       <c r="BA31" s="178"/>
     </row>
     <row r="32" spans="1:53" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="225"/>
+      <c r="A32" s="228"/>
       <c r="B32" s="108"/>
       <c r="C32" s="88" t="s">
         <v>103</v>
@@ -17335,7 +17378,7 @@
       <c r="BA32" s="178"/>
     </row>
     <row r="33" spans="1:57" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="225"/>
+      <c r="A33" s="228"/>
       <c r="B33" s="108"/>
       <c r="C33" s="87" t="s">
         <v>161</v>
@@ -17466,7 +17509,7 @@
       <c r="BE33" s="98"/>
     </row>
     <row r="34" spans="1:57" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="225"/>
+      <c r="A34" s="228"/>
       <c r="B34" s="108"/>
       <c r="C34" s="88" t="s">
         <v>445</v>
@@ -17597,7 +17640,7 @@
       <c r="BE34" s="98"/>
     </row>
     <row r="35" spans="1:57" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="225"/>
+      <c r="A35" s="228"/>
       <c r="B35" s="108"/>
       <c r="C35" s="88" t="s">
         <v>447</v>
@@ -17728,7 +17771,7 @@
       <c r="BE35" s="98"/>
     </row>
     <row r="36" spans="1:57" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="225"/>
+      <c r="A36" s="228"/>
       <c r="B36" s="108"/>
       <c r="C36" s="88" t="s">
         <v>177</v>
@@ -17859,7 +17902,7 @@
       <c r="BE36" s="98"/>
     </row>
     <row r="37" spans="1:57" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="225"/>
+      <c r="A37" s="228"/>
       <c r="B37" s="108"/>
       <c r="C37" s="88" t="s">
         <v>179</v>
@@ -17990,7 +18033,7 @@
       <c r="BE37" s="98"/>
     </row>
     <row r="38" spans="1:57" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="225"/>
+      <c r="A38" s="228"/>
       <c r="B38" s="108"/>
       <c r="C38" s="88" t="s">
         <v>180</v>
@@ -18121,7 +18164,7 @@
       <c r="BE38" s="98"/>
     </row>
     <row r="39" spans="1:57" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="225"/>
+      <c r="A39" s="228"/>
       <c r="B39" s="108"/>
       <c r="C39" s="86" t="s">
         <v>448</v>
@@ -18243,7 +18286,7 @@
       <c r="BA39" s="178"/>
     </row>
     <row r="40" spans="1:57" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="225"/>
+      <c r="A40" s="228"/>
       <c r="B40" s="108"/>
       <c r="C40" s="86" t="s">
         <v>149</v>
@@ -18371,7 +18414,7 @@
       <c r="BA40" s="179"/>
     </row>
     <row r="41" spans="1:57" s="86" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="226"/>
+      <c r="A41" s="229"/>
       <c r="B41" s="108"/>
       <c r="C41" s="88" t="s">
         <v>63</v>
@@ -18499,7 +18542,7 @@
       <c r="BA41" s="179"/>
     </row>
     <row r="42" spans="1:57" s="170" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="212" t="s">
+      <c r="A42" s="215" t="s">
         <v>483</v>
       </c>
       <c r="B42" s="166"/>
@@ -18628,7 +18671,7 @@
       <c r="BA42" s="180"/>
     </row>
     <row r="43" spans="1:57" s="78" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="213"/>
+      <c r="A43" s="216"/>
       <c r="B43" s="163"/>
       <c r="C43" s="91"/>
       <c r="D43" s="198" t="s">
@@ -18755,7 +18798,7 @@
       <c r="BA43" s="181"/>
     </row>
     <row r="44" spans="1:57" s="78" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="213"/>
+      <c r="A44" s="216"/>
       <c r="B44" s="163"/>
       <c r="C44" s="91"/>
       <c r="D44" s="198" t="s">
@@ -18881,7 +18924,7 @@
       <c r="BA44" s="181"/>
     </row>
     <row r="45" spans="1:57" s="78" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="213"/>
+      <c r="A45" s="216"/>
       <c r="B45" s="163"/>
       <c r="C45" s="91"/>
       <c r="D45" s="198" t="s">
@@ -19007,7 +19050,7 @@
       <c r="BA45" s="181"/>
     </row>
     <row r="46" spans="1:57" s="78" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="214"/>
+      <c r="A46" s="217"/>
       <c r="B46" s="163"/>
       <c r="C46" s="91"/>
       <c r="D46" s="198" t="s">
@@ -19259,7 +19302,7 @@
       <c r="BA47" s="181"/>
     </row>
     <row r="48" spans="1:57" s="154" customFormat="1" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="209" t="s">
+      <c r="A48" s="212" t="s">
         <v>482</v>
       </c>
       <c r="B48" s="153"/>
@@ -19386,7 +19429,7 @@
       <c r="BA48" s="182"/>
     </row>
     <row r="49" spans="1:53" s="154" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="210"/>
+      <c r="A49" s="213"/>
       <c r="B49" s="153"/>
       <c r="C49" s="154" t="s">
         <v>457</v>
@@ -19514,7 +19557,7 @@
       <c r="BA49" s="182"/>
     </row>
     <row r="50" spans="1:53" s="160" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="210"/>
+      <c r="A50" s="213"/>
       <c r="B50" s="153"/>
       <c r="C50" s="158" t="s">
         <v>457</v>
@@ -19641,7 +19684,7 @@
       <c r="BA50" s="183"/>
     </row>
     <row r="51" spans="1:53" s="160" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="210"/>
+      <c r="A51" s="213"/>
       <c r="B51" s="153"/>
       <c r="C51" s="158" t="s">
         <v>457</v>
@@ -19768,7 +19811,7 @@
       <c r="BA51" s="183"/>
     </row>
     <row r="52" spans="1:53" s="160" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="210"/>
+      <c r="A52" s="213"/>
       <c r="B52" s="153"/>
       <c r="C52" s="160" t="s">
         <v>457</v>
@@ -19891,7 +19934,7 @@
       <c r="BA52" s="183"/>
     </row>
     <row r="53" spans="1:53" s="160" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="210"/>
+      <c r="A53" s="213"/>
       <c r="B53" s="153"/>
       <c r="C53" s="160" t="s">
         <v>457</v>
@@ -20014,7 +20057,7 @@
       <c r="BA53" s="183"/>
     </row>
     <row r="54" spans="1:53" s="160" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="210"/>
+      <c r="A54" s="213"/>
       <c r="B54" s="153"/>
       <c r="C54" s="160" t="s">
         <v>457</v>
@@ -20137,7 +20180,7 @@
       <c r="BA54" s="183"/>
     </row>
     <row r="55" spans="1:53" s="160" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="210"/>
+      <c r="A55" s="213"/>
       <c r="B55" s="153"/>
       <c r="C55" s="158" t="s">
         <v>457</v>
@@ -20264,7 +20307,7 @@
       <c r="BA55" s="183"/>
     </row>
     <row r="56" spans="1:53" s="160" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="210"/>
+      <c r="A56" s="213"/>
       <c r="B56" s="153"/>
       <c r="C56" s="160" t="s">
         <v>457</v>
@@ -20386,7 +20429,7 @@
       <c r="BA56" s="183"/>
     </row>
     <row r="57" spans="1:53" s="160" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="210"/>
+      <c r="A57" s="213"/>
       <c r="B57" s="153"/>
       <c r="C57" s="160" t="s">
         <v>457</v>
@@ -20508,7 +20551,7 @@
       <c r="BA57" s="183"/>
     </row>
     <row r="58" spans="1:53" s="160" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="210"/>
+      <c r="A58" s="213"/>
       <c r="B58" s="153"/>
       <c r="C58" s="160" t="s">
         <v>457</v>
@@ -20630,7 +20673,7 @@
       <c r="BA58" s="183"/>
     </row>
     <row r="59" spans="1:53" s="160" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="210"/>
+      <c r="A59" s="213"/>
       <c r="B59" s="153"/>
       <c r="C59" s="160" t="s">
         <v>457</v>
@@ -20752,7 +20795,7 @@
       <c r="BA59" s="183"/>
     </row>
     <row r="60" spans="1:53" s="160" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="210"/>
+      <c r="A60" s="213"/>
       <c r="B60" s="153"/>
       <c r="C60" s="160" t="s">
         <v>457</v>
@@ -20880,7 +20923,7 @@
       <c r="BA60" s="184"/>
     </row>
     <row r="61" spans="1:53" s="160" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="211"/>
+      <c r="A61" s="214"/>
       <c r="B61" s="153"/>
       <c r="C61" s="160" t="s">
         <v>457</v>
@@ -22676,7 +22719,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="59" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="236" t="s">
         <v>60</v>
       </c>
       <c r="B1" s="55" t="s">
@@ -22701,7 +22744,7 @@
       <c r="I1" s="58"/>
     </row>
     <row r="2" spans="1:13" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="234"/>
+      <c r="A2" s="237"/>
       <c r="B2" s="41" t="s">
         <v>260</v>
       </c>
@@ -22722,7 +22765,7 @@
       <c r="I2" s="42"/>
     </row>
     <row r="3" spans="1:13" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="234"/>
+      <c r="A3" s="237"/>
       <c r="B3" s="41" t="s">
         <v>61</v>
       </c>
@@ -22741,7 +22784,7 @@
       <c r="I3" s="43"/>
     </row>
     <row r="4" spans="1:13" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="234"/>
+      <c r="A4" s="237"/>
       <c r="B4" s="41" t="s">
         <v>262</v>
       </c>
@@ -22760,7 +22803,7 @@
       <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:13" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="234"/>
+      <c r="A5" s="237"/>
       <c r="B5" s="41" t="s">
         <v>264</v>
       </c>
@@ -22781,7 +22824,7 @@
       <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:13" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="234"/>
+      <c r="A6" s="237"/>
       <c r="B6" s="41" t="s">
         <v>266</v>
       </c>
@@ -22807,7 +22850,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="234"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="41" t="s">
         <v>269</v>
       </c>
@@ -22833,7 +22876,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="234"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="41" t="s">
         <v>271</v>
       </c>
@@ -22857,7 +22900,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="234"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="41" t="s">
         <v>66</v>
       </c>
@@ -22878,7 +22921,7 @@
       <c r="L9" s="146"/>
     </row>
     <row r="10" spans="1:13" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="234"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="41" t="s">
         <v>71</v>
       </c>
@@ -22897,7 +22940,7 @@
       <c r="I10" s="43"/>
     </row>
     <row r="11" spans="1:13" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="234"/>
+      <c r="A11" s="237"/>
       <c r="B11" s="41" t="s">
         <v>75</v>
       </c>
@@ -22916,7 +22959,7 @@
       <c r="I11" s="43"/>
     </row>
     <row r="12" spans="1:13" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="234"/>
+      <c r="A12" s="237"/>
       <c r="B12" s="41" t="s">
         <v>275</v>
       </c>
@@ -22931,7 +22974,7 @@
       <c r="I12" s="42"/>
     </row>
     <row r="13" spans="1:13" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="234"/>
+      <c r="A13" s="237"/>
       <c r="B13" s="41" t="s">
         <v>79</v>
       </c>
@@ -22950,7 +22993,7 @@
       <c r="I13" s="43"/>
     </row>
     <row r="14" spans="1:13" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="234"/>
+      <c r="A14" s="237"/>
       <c r="B14" s="41" t="s">
         <v>277</v>
       </c>
@@ -22969,7 +23012,7 @@
       <c r="I14" s="45"/>
     </row>
     <row r="15" spans="1:13" s="40" customFormat="1" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="235"/>
+      <c r="A15" s="238"/>
       <c r="B15" s="46" t="s">
         <v>83</v>
       </c>
@@ -22988,7 +23031,7 @@
       <c r="I15" s="43"/>
     </row>
     <row r="16" spans="1:13" s="59" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="230" t="s">
+      <c r="A16" s="233" t="s">
         <v>281</v>
       </c>
       <c r="B16" s="60" t="s">
@@ -23007,7 +23050,7 @@
       <c r="I16" s="57"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="231"/>
+      <c r="A17" s="234"/>
       <c r="B17" s="47" t="s">
         <v>282</v>
       </c>
@@ -23026,7 +23069,7 @@
       <c r="I17" s="42"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="231"/>
+      <c r="A18" s="234"/>
       <c r="B18" s="47" t="s">
         <v>284</v>
       </c>
@@ -23045,7 +23088,7 @@
       <c r="I18" s="42"/>
     </row>
     <row r="19" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="231"/>
+      <c r="A19" s="234"/>
       <c r="B19" s="47" t="s">
         <v>286</v>
       </c>
@@ -23064,7 +23107,7 @@
       <c r="I19" s="42"/>
     </row>
     <row r="20" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="231"/>
+      <c r="A20" s="234"/>
       <c r="B20" s="47" t="s">
         <v>288</v>
       </c>
@@ -23083,7 +23126,7 @@
       <c r="I20" s="42"/>
     </row>
     <row r="21" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="232"/>
+      <c r="A21" s="235"/>
       <c r="B21" s="48" t="s">
         <v>290</v>
       </c>
@@ -23102,7 +23145,7 @@
       <c r="I21" s="42"/>
     </row>
     <row r="22" spans="1:9" s="59" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="236" t="s">
+      <c r="A22" s="239" t="s">
         <v>85</v>
       </c>
       <c r="B22" s="63" t="s">
@@ -23121,7 +23164,7 @@
       <c r="I22" s="57"/>
     </row>
     <row r="23" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="237"/>
+      <c r="A23" s="240"/>
       <c r="B23" s="49" t="s">
         <v>86</v>
       </c>
@@ -23142,7 +23185,7 @@
       <c r="I23" s="43"/>
     </row>
     <row r="24" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="237"/>
+      <c r="A24" s="240"/>
       <c r="B24" s="49" t="s">
         <v>89</v>
       </c>
@@ -23159,7 +23202,7 @@
       <c r="I24" s="43"/>
     </row>
     <row r="25" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="237"/>
+      <c r="A25" s="240"/>
       <c r="B25" s="49" t="s">
         <v>292</v>
       </c>
@@ -23176,7 +23219,7 @@
       <c r="I25" s="42"/>
     </row>
     <row r="26" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="237"/>
+      <c r="A26" s="240"/>
       <c r="B26" s="49" t="s">
         <v>294</v>
       </c>
@@ -23195,7 +23238,7 @@
       <c r="I26" s="42"/>
     </row>
     <row r="27" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="237"/>
+      <c r="A27" s="240"/>
       <c r="B27" s="49" t="s">
         <v>297</v>
       </c>
@@ -23212,7 +23255,7 @@
       <c r="I27" s="45"/>
     </row>
     <row r="28" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="237"/>
+      <c r="A28" s="240"/>
       <c r="B28" s="49" t="s">
         <v>91</v>
       </c>
@@ -23229,7 +23272,7 @@
       <c r="I28" s="43"/>
     </row>
     <row r="29" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="237"/>
+      <c r="A29" s="240"/>
       <c r="B29" s="49" t="s">
         <v>93</v>
       </c>
@@ -23246,7 +23289,7 @@
       <c r="I29" s="43"/>
     </row>
     <row r="30" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="237"/>
+      <c r="A30" s="240"/>
       <c r="B30" s="49" t="s">
         <v>95</v>
       </c>
@@ -23263,7 +23306,7 @@
       <c r="I30" s="43"/>
     </row>
     <row r="31" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="238"/>
+      <c r="A31" s="241"/>
       <c r="B31" s="50" t="s">
         <v>98</v>
       </c>
@@ -23284,7 +23327,7 @@
       <c r="I31" s="43"/>
     </row>
     <row r="32" spans="1:9" s="59" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="239" t="s">
+      <c r="A32" s="242" t="s">
         <v>299</v>
       </c>
       <c r="B32" s="66" t="s">
@@ -23303,7 +23346,7 @@
       <c r="I32" s="57"/>
     </row>
     <row r="33" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="240"/>
+      <c r="A33" s="243"/>
       <c r="B33" s="51" t="s">
         <v>300</v>
       </c>
@@ -23318,7 +23361,7 @@
       <c r="I33" s="42"/>
     </row>
     <row r="34" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="240"/>
+      <c r="A34" s="243"/>
       <c r="B34" s="51" t="s">
         <v>302</v>
       </c>
@@ -23333,7 +23376,7 @@
       <c r="I34" s="42"/>
     </row>
     <row r="35" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="240"/>
+      <c r="A35" s="243"/>
       <c r="B35" s="51" t="s">
         <v>304</v>
       </c>
@@ -23348,7 +23391,7 @@
       <c r="I35" s="42"/>
     </row>
     <row r="36" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="240"/>
+      <c r="A36" s="243"/>
       <c r="B36" s="51" t="s">
         <v>306</v>
       </c>
@@ -23363,7 +23406,7 @@
       <c r="I36" s="42"/>
     </row>
     <row r="37" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="241"/>
+      <c r="A37" s="244"/>
       <c r="B37" s="52" t="s">
         <v>308</v>
       </c>
@@ -23378,7 +23421,7 @@
       <c r="I37" s="42"/>
     </row>
     <row r="38" spans="1:9" s="59" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="227" t="s">
+      <c r="A38" s="230" t="s">
         <v>100</v>
       </c>
       <c r="B38" s="69" t="s">
@@ -23397,7 +23440,7 @@
       <c r="I38" s="57"/>
     </row>
     <row r="39" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="228"/>
+      <c r="A39" s="231"/>
       <c r="B39" s="53" t="s">
         <v>101</v>
       </c>
@@ -23416,7 +23459,7 @@
       <c r="I39" s="43"/>
     </row>
     <row r="40" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="228"/>
+      <c r="A40" s="231"/>
       <c r="B40" s="53" t="s">
         <v>104</v>
       </c>
@@ -23435,7 +23478,7 @@
       <c r="I40" s="43"/>
     </row>
     <row r="41" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="228"/>
+      <c r="A41" s="231"/>
       <c r="B41" s="53" t="s">
         <v>108</v>
       </c>
@@ -23454,7 +23497,7 @@
       <c r="I41" s="43"/>
     </row>
     <row r="42" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="228"/>
+      <c r="A42" s="231"/>
       <c r="B42" s="53" t="s">
         <v>110</v>
       </c>
@@ -23473,7 +23516,7 @@
       <c r="I42" s="43"/>
     </row>
     <row r="43" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="228"/>
+      <c r="A43" s="231"/>
       <c r="B43" s="53" t="s">
         <v>66</v>
       </c>
@@ -23490,7 +23533,7 @@
       <c r="I43" s="43"/>
     </row>
     <row r="44" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="228"/>
+      <c r="A44" s="231"/>
       <c r="B44" s="53" t="s">
         <v>113</v>
       </c>
@@ -23507,7 +23550,7 @@
       <c r="I44" s="43"/>
     </row>
     <row r="45" spans="1:9" s="40" customFormat="1" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="229"/>
+      <c r="A45" s="232"/>
       <c r="B45" s="54" t="s">
         <v>312</v>
       </c>
@@ -23565,54 +23608,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="248" t="s">
         <v>328</v>
       </c>
-      <c r="B1" s="246"/>
-      <c r="C1" s="246"/>
-      <c r="D1" s="246"/>
-      <c r="E1" s="246"/>
-      <c r="F1" s="246"/>
-      <c r="G1" s="246"/>
-      <c r="H1" s="246"/>
-      <c r="I1" s="246"/>
-      <c r="J1" s="246"/>
-      <c r="K1" s="246"/>
-      <c r="L1" s="246"/>
-      <c r="M1" s="246"/>
-      <c r="N1" s="246"/>
-      <c r="O1" s="246"/>
-      <c r="P1" s="246"/>
-      <c r="Q1" s="246"/>
-      <c r="R1" s="246"/>
-      <c r="S1" s="246"/>
-      <c r="T1" s="246"/>
-      <c r="U1" s="246"/>
+      <c r="B1" s="249"/>
+      <c r="C1" s="249"/>
+      <c r="D1" s="249"/>
+      <c r="E1" s="249"/>
+      <c r="F1" s="249"/>
+      <c r="G1" s="249"/>
+      <c r="H1" s="249"/>
+      <c r="I1" s="249"/>
+      <c r="J1" s="249"/>
+      <c r="K1" s="249"/>
+      <c r="L1" s="249"/>
+      <c r="M1" s="249"/>
+      <c r="N1" s="249"/>
+      <c r="O1" s="249"/>
+      <c r="P1" s="249"/>
+      <c r="Q1" s="249"/>
+      <c r="R1" s="249"/>
+      <c r="S1" s="249"/>
+      <c r="T1" s="249"/>
+      <c r="U1" s="249"/>
     </row>
     <row r="2" spans="1:21" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="244" t="s">
+      <c r="A2" s="247" t="s">
         <v>444</v>
       </c>
-      <c r="B2" s="244"/>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
-      <c r="J2" s="244"/>
-      <c r="K2" s="244"/>
-      <c r="L2" s="244"/>
-      <c r="M2" s="244"/>
-      <c r="N2" s="244"/>
-      <c r="O2" s="244"/>
-      <c r="P2" s="244"/>
-      <c r="Q2" s="244"/>
-      <c r="R2" s="244"/>
-      <c r="S2" s="244"/>
-      <c r="T2" s="244"/>
-      <c r="U2" s="244"/>
+      <c r="B2" s="247"/>
+      <c r="C2" s="247"/>
+      <c r="D2" s="247"/>
+      <c r="E2" s="247"/>
+      <c r="F2" s="247"/>
+      <c r="G2" s="247"/>
+      <c r="H2" s="247"/>
+      <c r="I2" s="247"/>
+      <c r="J2" s="247"/>
+      <c r="K2" s="247"/>
+      <c r="L2" s="247"/>
+      <c r="M2" s="247"/>
+      <c r="N2" s="247"/>
+      <c r="O2" s="247"/>
+      <c r="P2" s="247"/>
+      <c r="Q2" s="247"/>
+      <c r="R2" s="247"/>
+      <c r="S2" s="247"/>
+      <c r="T2" s="247"/>
+      <c r="U2" s="247"/>
     </row>
     <row r="3" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
@@ -23805,31 +23848,31 @@
       <c r="A6" s="83"/>
       <c r="B6" s="83"/>
       <c r="C6" s="83"/>
-      <c r="L6" s="243" t="s">
+      <c r="L6" s="246" t="s">
         <v>415</v>
       </c>
-      <c r="M6" s="243"/>
-      <c r="N6" s="243"/>
-      <c r="O6" s="243"/>
-      <c r="P6" s="243"/>
+      <c r="M6" s="246"/>
+      <c r="N6" s="246"/>
+      <c r="O6" s="246"/>
+      <c r="P6" s="246"/>
     </row>
     <row r="8" spans="1:21" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="242" t="s">
+      <c r="A8" s="245" t="s">
         <v>329</v>
       </c>
-      <c r="B8" s="242"/>
-      <c r="C8" s="242"/>
-      <c r="D8" s="242"/>
-      <c r="E8" s="242"/>
-      <c r="F8" s="242"/>
-      <c r="G8" s="242"/>
-      <c r="H8" s="242"/>
-      <c r="I8" s="242"/>
-      <c r="J8" s="242"/>
-      <c r="K8" s="242"/>
-      <c r="L8" s="242"/>
-      <c r="M8" s="242"/>
-      <c r="N8" s="242"/>
+      <c r="B8" s="245"/>
+      <c r="C8" s="245"/>
+      <c r="D8" s="245"/>
+      <c r="E8" s="245"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245"/>
+      <c r="H8" s="245"/>
+      <c r="I8" s="245"/>
+      <c r="J8" s="245"/>
+      <c r="K8" s="245"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="245"/>
+      <c r="N8" s="245"/>
     </row>
     <row r="9" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="79" t="s">

</xml_diff>